<commit_message>
feature: 모든 테이블에 대한 Service, Controller 구현
모든 테이블에 대한 Service, Controller 구현
의존성 주입(Dependency Injection, DI) 기능 수정.
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gj156\Desktop\Development\ERPSystem\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834E64E3-6446-4C58-AAF4-313030C2D044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EA4794-82B8-42E1-9C94-1106161DABCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{1A754DB6-FF10-4809-A0D2-9C6CDB9AA5B2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
   <si>
     <t>code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -568,7 +568,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -599,7 +599,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -648,7 +648,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="A1:C9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -980,23 +980,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6BB459-5620-4A1D-9826-E641F7D7F724}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A6:G45"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.125" customWidth="1"/>
+    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="D1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1">
         <v>0</v>
@@ -1018,8 +1018,11 @@
       <c r="G1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
@@ -1039,75 +1042,87 @@
         <v>28</v>
       </c>
       <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>33</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>34</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>35</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>25</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>94</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>100</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>200</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>300</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>20240601</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
         <v>346</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>34</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>141</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2341</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>421</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>20240602</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feature: ERPDataInitializer 기능 추가
enum 데이터 입력 기능 추가.
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gj156\Desktop\Development\ERPSystem\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EA4794-82B8-42E1-9C94-1106161DABCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C252EE7-383F-49CB-98C6-477720CEE829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{1A754DB6-FF10-4809-A0D2-9C6CDB9AA5B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{1A754DB6-FF10-4809-A0D2-9C6CDB9AA5B2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Entries" sheetId="1" r:id="rId1"/>
-    <sheet name="VatTypes" sheetId="2" r:id="rId2"/>
+    <sheet name="Entry" sheetId="1" r:id="rId1"/>
+    <sheet name="VatType" sheetId="2" r:id="rId2"/>
     <sheet name="CashBook" sheetId="3" r:id="rId3"/>
+    <sheet name="TaxInvoice" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
   <si>
     <t>code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -181,6 +182,109 @@
   </si>
   <si>
     <t>balance_forward</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vendor_code</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>issueStatus</t>
+  </si>
+  <si>
+    <t>ntsTransmissionStatus</t>
+  </si>
+  <si>
+    <t>issue_date</t>
+  </si>
+  <si>
+    <t>attachment_included</t>
+  </si>
+  <si>
+    <t>item_description</t>
+  </si>
+  <si>
+    <t>supply_value</t>
+  </si>
+  <si>
+    <t>tax_amount</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>bigdecimal</t>
+  </si>
+  <si>
+    <t>VC001</t>
+  </si>
+  <si>
+    <t>제품 설명</t>
+  </si>
+  <si>
+    <t>VC002</t>
+  </si>
+  <si>
+    <t>서비스 설명</t>
+  </si>
+  <si>
+    <t>approval_number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RECEIPT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReceiptType</t>
+  </si>
+  <si>
+    <t>receiptType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INVOICE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IssueStatus</t>
+  </si>
+  <si>
+    <t>THIRD_PARTY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELF_ISSUED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NTSStatus</t>
+  </si>
+  <si>
+    <t>TRANSMITTED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PENDING</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TaxType</t>
+  </si>
+  <si>
+    <t>TAXABLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXEMPT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -205,20 +309,41 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -227,9 +352,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -568,72 +699,72 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -648,327 +779,327 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>15</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>17</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>19</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>20</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>21</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>22</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>24</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>25</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>26</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -982,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6BB459-5620-4A1D-9826-E641F7D7F724}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -997,133 +1128,353 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
         <v>25</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>94</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>100</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>200</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>300</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>20240601</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>346</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>34</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>141</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>2341</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>421</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>20240602</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB35329-EBCD-46FF-8FF6-8B0ADEB759EB}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1" s="2">
+        <v>0</v>
+      </c>
+      <c r="K1" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="1">
+        <v>20240601</v>
+      </c>
+      <c r="H4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K4" s="1">
+        <v>100000</v>
+      </c>
+      <c r="L4" s="1">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="1">
+        <v>20240602</v>
+      </c>
+      <c r="H5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="1">
+        <v>500000</v>
+      </c>
+      <c r="K5" s="1">
+        <v>50000</v>
+      </c>
+      <c r="L5" s="1">
+        <v>987654321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: ERPDataInitializer 기능 수정
빌더패턴에 적용되도록 ERPDataInitializer 기능 수정
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gj156\Desktop\Development\ERPSystem\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C252EE7-383F-49CB-98C6-477720CEE829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E7DC95-F166-4FEA-8CE6-3594B72FC7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{1A754DB6-FF10-4809-A0D2-9C6CDB9AA5B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1A754DB6-FF10-4809-A0D2-9C6CDB9AA5B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Entry" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="64">
   <si>
     <t>code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -188,9 +188,6 @@
     <t>vendor_code</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>issueStatus</t>
   </si>
   <si>
@@ -240,51 +237,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RECEIPT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReceiptType</t>
-  </si>
-  <si>
     <t>receiptType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>INVOICE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IssueStatus</t>
-  </si>
-  <si>
-    <t>THIRD_PARTY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELF_ISSUED</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NTSStatus</t>
-  </si>
-  <si>
-    <t>TRANSMITTED</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PENDING</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TaxType</t>
-  </si>
-  <si>
-    <t>TAXABLE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXEMPT</t>
+    <t>enum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TaxType.TAXABLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TaxType.EXEMPT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReceiptType.RECEIPT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReceiptType.INVOICE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IssueStatus.THIRD_PARTY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IssueStatus.SELF_ISSUED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NTSStatus.TRANSMITTED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NTSStatus.PENDING</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>taxType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -696,75 +689,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6829820-5163-451C-BDE8-9004A047D6C2}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="1">
         <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -776,330 +761,319 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9BEFEAC-7826-45BE-81E0-0B8E7BEEC07A}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D24" sqref="D24:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="1">
         <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>26</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1111,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6BB459-5620-4A1D-9826-E641F7D7F724}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1128,132 +1102,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2">
-        <v>0</v>
-      </c>
-      <c r="F1" s="2">
-        <v>0</v>
-      </c>
-      <c r="G1" s="2">
-        <v>0</v>
-      </c>
-      <c r="H1" s="2">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>29</v>
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1">
+        <v>94</v>
+      </c>
+      <c r="E3" s="1">
+        <v>100</v>
+      </c>
+      <c r="F3" s="1">
+        <v>200</v>
+      </c>
+      <c r="G3" s="1">
+        <v>300</v>
+      </c>
+      <c r="H3" s="1">
+        <v>20240601</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>25</v>
+        <v>346</v>
       </c>
       <c r="D4" s="1">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="F4" s="1">
-        <v>200</v>
+        <v>2341</v>
       </c>
       <c r="G4" s="1">
-        <v>300</v>
+        <v>421</v>
       </c>
       <c r="H4" s="1">
-        <v>20240601</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>346</v>
-      </c>
-      <c r="D5" s="1">
-        <v>34</v>
-      </c>
-      <c r="E5" s="1">
-        <v>141</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2341</v>
-      </c>
-      <c r="G5" s="1">
-        <v>421</v>
-      </c>
-      <c r="H5" s="1">
         <v>20240602</v>
       </c>
     </row>
@@ -1265,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB35329-EBCD-46FF-8FF6-8B0ADEB759EB}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1276,8 +1224,7 @@
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="24.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
@@ -1288,192 +1235,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="2">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2">
-        <v>0</v>
-      </c>
-      <c r="F1" s="2">
-        <v>0</v>
-      </c>
-      <c r="G1" s="2">
-        <v>0</v>
-      </c>
-      <c r="H1" s="2">
-        <v>0</v>
-      </c>
-      <c r="I1" s="2">
-        <v>0</v>
-      </c>
-      <c r="J1" s="2">
-        <v>0</v>
-      </c>
-      <c r="K1" s="2">
-        <v>0</v>
-      </c>
-      <c r="L1" s="2">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>53</v>
+      <c r="G3" s="1">
+        <v>20240601</v>
+      </c>
+      <c r="H3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K3" s="1">
+        <v>100000</v>
+      </c>
+      <c r="L3" s="1">
+        <v>123456789</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>62</v>
       </c>
       <c r="G4" s="1">
-        <v>20240601</v>
+        <v>20240602</v>
       </c>
       <c r="H4" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J4" s="1">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="K4" s="1">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="L4" s="1">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" s="1">
-        <v>20240602</v>
-      </c>
-      <c r="H5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" s="1">
-        <v>500000</v>
-      </c>
-      <c r="K5" s="1">
-        <v>50000</v>
-      </c>
-      <c r="L5" s="1">
         <v>987654321</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feature: 각엔티티별 code, id 통합 및 NotNull 적용
각엔티티별 code, id 통합 및 NotNull 적용
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gj156\Desktop\Development\ERPSystem\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga31\Desktop\수업\3. IntelliJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC0AEA1-9FE1-4054-9B61-92381FFEF745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685EA437-3EC8-47CE-80B0-9A0CF26503E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{1A754DB6-FF10-4809-A0D2-9C6CDB9AA5B2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{1A754DB6-FF10-4809-A0D2-9C6CDB9AA5B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Entry" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,11 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="63">
-  <si>
-    <t>code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -236,18 +230,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>transactionCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>memosCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vendorCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>balanceForward</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -281,6 +263,18 @@
   </si>
   <si>
     <t>LocalDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transactionId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memosId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vendorId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -698,68 +692,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6829820-5163-451C-BDE8-9004A047D6C2}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -770,320 +743,236 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9BEFEAC-7826-45BE-81E0-0B8E7BEEC07A}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:D25"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="1" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="1" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1094,304 +983,281 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6BB459-5620-4A1D-9826-E641F7D7F724}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.125" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="D3" s="1">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E3" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="F3" s="1">
-        <v>200</v>
-      </c>
-      <c r="G3" s="1">
         <v>300</v>
       </c>
-      <c r="H3" s="3">
+      <c r="G3" s="3">
         <v>45444</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>346</v>
       </c>
       <c r="C4" s="1">
-        <v>346</v>
+        <v>34</v>
       </c>
       <c r="D4" s="1">
-        <v>34</v>
+        <v>141</v>
       </c>
       <c r="E4" s="1">
-        <v>141</v>
+        <v>2341</v>
       </c>
       <c r="F4" s="1">
-        <v>2341</v>
-      </c>
-      <c r="G4" s="1">
         <v>421</v>
       </c>
-      <c r="H4" s="3">
+      <c r="G4" s="3">
         <v>45445</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB35329-EBCD-46FF-8FF6-8B0ADEB759EB}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="24.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="H1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="4">
+        <v>45445</v>
+      </c>
+      <c r="G3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="I3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="J3" s="1">
+        <v>100000</v>
+      </c>
+      <c r="K3" s="1">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="4">
-        <v>45445</v>
-      </c>
-      <c r="H3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="K3" s="1">
-        <v>100000</v>
-      </c>
-      <c r="L3" s="1">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="F4" s="4">
+        <v>45446</v>
+      </c>
+      <c r="G4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="4">
-        <v>45446</v>
-      </c>
-      <c r="H4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>40</v>
+      <c r="I4" s="1">
+        <v>500000</v>
       </c>
       <c r="J4" s="1">
-        <v>500000</v>
+        <v>50000</v>
       </c>
       <c r="K4" s="1">
-        <v>50000</v>
-      </c>
-      <c r="L4" s="1">
         <v>987654321</v>
       </c>
     </row>

</xml_diff>